<commit_message>
changement modele gradient boosting
</commit_message>
<xml_diff>
--- a/result_with_predictions.xlsx
+++ b/result_with_predictions.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -5030,7 +5030,7 @@
       </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -5180,7 +5180,7 @@
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -5330,7 +5330,7 @@
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -5780,7 +5780,7 @@
       </c>
       <c r="S71" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="S72" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -6830,7 +6830,7 @@
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -6905,7 +6905,7 @@
       </c>
       <c r="S86" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -8630,7 +8630,7 @@
       </c>
       <c r="S109" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -9080,7 +9080,7 @@
       </c>
       <c r="S115" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -9455,7 +9455,7 @@
       </c>
       <c r="S120" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -10055,7 +10055,7 @@
       </c>
       <c r="S128" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -10505,7 +10505,7 @@
       </c>
       <c r="S134" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -11855,7 +11855,7 @@
       </c>
       <c r="S152" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -15530,7 +15530,7 @@
       </c>
       <c r="S201" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -15980,7 +15980,7 @@
       </c>
       <c r="S207" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -16955,7 +16955,7 @@
       </c>
       <c r="S220" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -18755,7 +18755,7 @@
       </c>
       <c r="S244" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -19430,7 +19430,7 @@
       </c>
       <c r="S253" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -19580,7 +19580,7 @@
       </c>
       <c r="S255" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -20255,7 +20255,7 @@
       </c>
       <c r="S264" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -23330,7 +23330,7 @@
       </c>
       <c r="S305" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -23705,7 +23705,7 @@
       </c>
       <c r="S310" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -24680,7 +24680,7 @@
       </c>
       <c r="S323" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -24830,7 +24830,7 @@
       </c>
       <c r="S325" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -25355,7 +25355,7 @@
       </c>
       <c r="S332" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -25730,7 +25730,7 @@
       </c>
       <c r="S337" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -26630,7 +26630,7 @@
       </c>
       <c r="S349" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -28805,7 +28805,7 @@
       </c>
       <c r="S378" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -30305,7 +30305,7 @@
       </c>
       <c r="S398" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -30605,7 +30605,7 @@
       </c>
       <c r="S402" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -31205,7 +31205,7 @@
       </c>
       <c r="S410" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -32405,7 +32405,7 @@
       </c>
       <c r="S426" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -33230,7 +33230,7 @@
       </c>
       <c r="S437" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -33755,7 +33755,7 @@
       </c>
       <c r="S444" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -34355,7 +34355,7 @@
       </c>
       <c r="S452" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -34805,7 +34805,7 @@
       </c>
       <c r="S458" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -34880,7 +34880,7 @@
       </c>
       <c r="S459" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -36155,7 +36155,7 @@
       </c>
       <c r="S476" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -36455,7 +36455,7 @@
       </c>
       <c r="S480" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -37130,7 +37130,7 @@
       </c>
       <c r="S489" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -37205,7 +37205,7 @@
       </c>
       <c r="S490" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -38405,7 +38405,7 @@
       </c>
       <c r="S506" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -38855,7 +38855,7 @@
       </c>
       <c r="S512" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -39905,7 +39905,7 @@
       </c>
       <c r="S526" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -40505,7 +40505,7 @@
       </c>
       <c r="S534" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -41180,7 +41180,7 @@
       </c>
       <c r="S543" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -41480,7 +41480,7 @@
       </c>
       <c r="S547" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -42230,7 +42230,7 @@
       </c>
       <c r="S557" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -42680,7 +42680,7 @@
       </c>
       <c r="S563" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -43355,7 +43355,7 @@
       </c>
       <c r="S572" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -44255,7 +44255,7 @@
       </c>
       <c r="S584" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -44330,7 +44330,7 @@
       </c>
       <c r="S585" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -44705,7 +44705,7 @@
       </c>
       <c r="S590" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -45305,7 +45305,7 @@
       </c>
       <c r="S598" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -45530,7 +45530,7 @@
       </c>
       <c r="S601" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -45605,7 +45605,7 @@
       </c>
       <c r="S602" t="inlineStr">
         <is>
-          <t>négatif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -46130,7 +46130,7 @@
       </c>
       <c r="S609" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -48080,7 +48080,7 @@
       </c>
       <c r="S635" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -48605,7 +48605,7 @@
       </c>
       <c r="S642" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -48905,7 +48905,7 @@
       </c>
       <c r="S646" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -49205,7 +49205,7 @@
       </c>
       <c r="S650" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>négatif</t>
         </is>
       </c>
     </row>
@@ -49430,7 +49430,7 @@
       </c>
       <c r="S653" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -49655,7 +49655,7 @@
       </c>
       <c r="S656" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -50555,7 +50555,7 @@
       </c>
       <c r="S668" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>
@@ -51005,7 +51005,7 @@
       </c>
       <c r="S674" t="inlineStr">
         <is>
-          <t>neutre</t>
+          <t>positif</t>
         </is>
       </c>
     </row>
@@ -52955,7 +52955,7 @@
       </c>
       <c r="S700" t="inlineStr">
         <is>
-          <t>positif</t>
+          <t>neutre</t>
         </is>
       </c>
     </row>

</xml_diff>